<commit_message>
updated data after match no: 4
</commit_message>
<xml_diff>
--- a/matchInfo.xlsx
+++ b/matchInfo.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="52">
   <si>
     <t>slno</t>
   </si>
@@ -58,6 +58,9 @@
     <t>mom</t>
   </si>
   <si>
+    <t>team</t>
+  </si>
+  <si>
     <t>09.04.2021</t>
   </si>
   <si>
@@ -143,6 +146,27 @@
   </si>
   <si>
     <t>Nitish Rana</t>
+  </si>
+  <si>
+    <t>12.04.2021</t>
+  </si>
+  <si>
+    <t>PBKS</t>
+  </si>
+  <si>
+    <t>RR</t>
+  </si>
+  <si>
+    <t>KL Rahul</t>
+  </si>
+  <si>
+    <t>Sanju Samson</t>
+  </si>
+  <si>
+    <t>221 - 6</t>
+  </si>
+  <si>
+    <t>217 - 7</t>
   </si>
 </sst>
 </file>
@@ -459,6 +483,9 @@
       <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="P1" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2">
@@ -468,43 +495,46 @@
         <v>1.0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="K2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L2" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="L2" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="M2" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="3">
@@ -515,43 +545,46 @@
         <v>2.0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="I3" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="K3" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="4">
@@ -562,43 +595,46 @@
         <v>3.0</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="N4" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="J4" s="2" t="s">
+      <c r="O4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="P4" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="5">
@@ -606,6 +642,51 @@
         <f t="shared" ref="A5:A61" si="1">(A4+1)</f>
         <v>4</v>
       </c>
+      <c r="B5" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="2">

</xml_diff>